<commit_message>
Changes to datafiles to change dsm calculation from stock to all inflow driven. Changes to Config file and data files to include appliances in python script
</commit_message>
<xml_diff>
--- a/Data/2_S_RECC_FinalProducts_2015_appliances_V1.0.xlsx
+++ b/Data/2_S_RECC_FinalProducts_2015_appliances_V1.0.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14276" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14276" uniqueCount="95">
   <si>
     <t>ODYM-RECC Parameter File</t>
   </si>
@@ -265,9 +265,6 @@
     <t>Mean lifetime</t>
   </si>
   <si>
-    <t>good g</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
@@ -302,6 +299,12 @@
   </si>
   <si>
     <t>Stats_array_string</t>
+  </si>
+  <si>
+    <t>Appliances a</t>
+  </si>
+  <si>
+    <t>Sector_appliances</t>
   </si>
 </sst>
 </file>
@@ -731,7 +734,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,13 +1083,13 @@
         <v>46</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>1</v>
@@ -1106,10 +1109,10 @@
         <v>46</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>51</v>
@@ -1129,13 +1132,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>53</v>
@@ -1155,10 +1158,10 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>89</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>90</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -1175,10 +1178,10 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -1222,7 +1225,7 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C31" s="13"/>
       <c r="D31" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
@@ -1285,10 +1288,10 @@
         <v>46</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>89</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>47</v>
@@ -1297,13 +1300,13 @@
         <v>55</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>